<commit_message>
ok letzter pusch nochmal zeitplanung aktualisiert
</commit_message>
<xml_diff>
--- a/docs/Krystian-Usarz-Zeitplanung.xlsx
+++ b/docs/Krystian-Usarz-Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ACW\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A62B5179-AC5D-45BD-8790-0DDFC4F66BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E2E601-310D-4F2C-8818-4636EC9B84F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1959,7 +1959,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.5</c:v>
+                  <c:v>26.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2466,8 +2466,8 @@
   </sheetPr>
   <dimension ref="A1:BJ45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y48" sqref="Y48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3753,7 +3753,7 @@
       </c>
       <c r="D18" s="41">
         <f>SUM(D19:D33)</f>
-        <v>18.5</v>
+        <v>26.5</v>
       </c>
       <c r="E18" s="31"/>
       <c r="F18" s="30"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="D23" s="80">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E23" s="49">
         <v>1</v>
@@ -4160,7 +4160,9 @@
       <c r="T23" s="57"/>
       <c r="U23" s="112"/>
       <c r="V23" s="59"/>
-      <c r="W23" s="115"/>
+      <c r="W23" s="115">
+        <v>6</v>
+      </c>
       <c r="X23" s="60"/>
       <c r="Y23" s="55"/>
       <c r="Z23" s="56"/>
@@ -4515,7 +4517,7 @@
       </c>
       <c r="D28" s="80">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E28" s="49">
         <v>2</v>
@@ -4537,7 +4539,9 @@
       <c r="T28" s="57"/>
       <c r="U28" s="58"/>
       <c r="V28" s="59"/>
-      <c r="W28" s="115"/>
+      <c r="W28" s="115">
+        <v>2</v>
+      </c>
       <c r="X28" s="115"/>
       <c r="Y28" s="108"/>
       <c r="Z28" s="56"/>
@@ -5752,7 +5756,7 @@
       </c>
       <c r="D45" s="36">
         <f>D41+D38+D34+D18+D14+D9</f>
-        <v>24.5</v>
+        <v>32.5</v>
       </c>
       <c r="E45" s="36"/>
       <c r="F45" s="37"/>
@@ -5822,7 +5826,7 @@
       </c>
       <c r="W45" s="38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X45" s="38">
         <f t="shared" si="4"/>
@@ -6096,7 +6100,7 @@
       </c>
       <c r="D5" s="77">
         <f>Zeitplanung!D18</f>
-        <v>18.5</v>
+        <v>26.5</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="78"/>

</xml_diff>